<commit_message>
lit review XLSX file, updated reduced risk section: Gamba, Harris, Joosse, and working on Curiel-Lewandrowski
</commit_message>
<xml_diff>
--- a/references/Lit review_NSAIDS melanoma.xlsx
+++ b/references/Lit review_NSAIDS melanoma.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REB\AARP_HRTandMelanoma\Analysis\references\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\REB\NSAIDS melanoma AARP\Analysis\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,14 +18,14 @@
     <sheet name="strengths.limitations" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lit Review'!$A$1:$K$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lit Review'!$A$1:$M$20</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="155">
   <si>
     <t>Study type</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Cancer</t>
   </si>
   <si>
-    <t>Women's Health Initiative; USA</t>
-  </si>
-  <si>
     <t>cohort</t>
   </si>
   <si>
@@ -186,33 +183,12 @@
     <t>all nsaids</t>
   </si>
   <si>
-    <t>conclusion</t>
-  </si>
-  <si>
-    <t>limitations</t>
-  </si>
-  <si>
-    <t>results not stratified by drug type</t>
-  </si>
-  <si>
-    <t>1318 cases, 6786 control</t>
-  </si>
-  <si>
     <t>both</t>
   </si>
   <si>
-    <t>study population (n)</t>
-  </si>
-  <si>
     <t>aspirin and other nsaids</t>
   </si>
   <si>
-    <t>reduced risk in females with consistent low-dose aspirin</t>
-  </si>
-  <si>
-    <t>3242 melanoma cases, 1974 SCC cases, 178,655 controls</t>
-  </si>
-  <si>
     <t>reduced risk of SCC and malignant melanoma with different NSAID use; greater risk reduction with greater duration and dosage of NSAID use</t>
   </si>
   <si>
@@ -222,9 +198,6 @@
     <t>aspirin</t>
   </si>
   <si>
-    <t>21% reduced risk of melanoma with aspirin use; 30% reduced melanoma risk with aspirin use &gt;5 yrs</t>
-  </si>
-  <si>
     <t>no info on family hx of skin cancer</t>
   </si>
   <si>
@@ -267,15 +240,9 @@
     <t>review</t>
   </si>
   <si>
-    <t>RCT</t>
-  </si>
-  <si>
     <t>100mg of aspirin may be insufficient dose; insufficient follow-up time (10 years)</t>
   </si>
   <si>
-    <t>no association; nsaid use (HR 1.12; 9% CI 0.84-1.48), regular or extra strength (HR 1.22; 95%CI 0.76-1.58), non-aspirin NSAIDS (HR1.22; 95% CI 0.75-1.99)</t>
-  </si>
-  <si>
     <t>exposure time (within past 10 years) may have been too short</t>
   </si>
   <si>
@@ -291,12 +258,6 @@
     <t>Reviews/meta-analyses</t>
   </si>
   <si>
-    <t>39876. 100 mg aspirin every other day (19934) placebo (19942)</t>
-  </si>
-  <si>
-    <t>no association. 68 cases on aspirin, 70 cases on placebo, RR=0.97 (0.70-1.36)</t>
-  </si>
-  <si>
     <t>Cook, 2005</t>
   </si>
   <si>
@@ -312,15 +273,9 @@
     <t>constitutional characteristics/individual level risk factors</t>
   </si>
   <si>
-    <t>reduced risk in both genders with long-term aspirin use</t>
-  </si>
-  <si>
     <t>cutaneous melanoma cases determined through dermatology clinics assoc with dana Farber Harvard Cancer Center. Age, gender, town matched community controls</t>
   </si>
   <si>
-    <t xml:space="preserve">never exposed and &lt;2 years were combined because &lt;2 years exposure likely to not have effect on CM carcinogenesis and in prelim analysis showed no difference with never exposed on CM risk. </t>
-  </si>
-  <si>
     <t>Zhu, 2015</t>
   </si>
   <si>
@@ -333,9 +288,6 @@
     <t>meta-analysis</t>
   </si>
   <si>
-    <t>11 published studies included. Pooled data exposure 50-400 mg aspirin intake associated with reduced risk of all skin cancer (OR 0.94 (0.90-0.99). Low-dose (&lt;150mg) reduce risk (OR 0.95 (0.90-0.99). NO association with MELANOMA (OR 0.96, 0.82-1.12) 7 studies had information on melanoma, but these were significantly heterogeneous (p=0.00)</t>
-  </si>
-  <si>
     <t>Joosse, 2009</t>
   </si>
   <si>
@@ -366,18 +318,12 @@
     <t>no ambient UVR adjustment</t>
   </si>
   <si>
-    <t xml:space="preserve">no association-- aspirin adjusted OR1.45 (0.44-4.74); non-aspirin NSAID adjusted OR 0.71 (0.23-2.02) -- adjusted for age, gnder, skin color, family hx of melanoma, # moles; COX-2 inhibitors OR 0.61 (0.28-1.31). </t>
-  </si>
-  <si>
     <t>structured interview and aspirin use have have been misreported, small numbers</t>
   </si>
   <si>
     <t>Nurses Health Study</t>
   </si>
   <si>
-    <t>increased risk of melanoma for current aspirin users (RR 1.32; 95%CI 1.03-1.70)</t>
-  </si>
-  <si>
     <t>Cutaneous Melanoma cases more likely to have light hair, eyes, number of freckles, skin response to sun and number of sunburns</t>
   </si>
   <si>
@@ -390,15 +336,9 @@
     <t>Cancer Prevention Study II Nutrition Cohort, 1992-2003</t>
   </si>
   <si>
-    <t>69810 men 76303 women, melanoma analysis combined genders</t>
-  </si>
-  <si>
     <t>"adult-strenght" aspirin (&gt;=325 mg/day</t>
   </si>
   <si>
-    <t>no association -- low dose RR 1.04 (0.88-1.22), current daily use (&lt;5 yr) RR 0.99 (0.79-1.25), current daily use (&gt;= 5yrs) RR 1.15 (0.83-1.59)</t>
-  </si>
-  <si>
     <t>did not adjust for constitutional risk factors (light hair/eyes)</t>
   </si>
   <si>
@@ -417,9 +357,6 @@
     <t>registry-based case-control (Denmark)</t>
   </si>
   <si>
-    <t>Dutch registry based</t>
-  </si>
-  <si>
     <t>Harris, 2001</t>
   </si>
   <si>
@@ -429,23 +366,540 @@
     <t>110 cases, 609 controls frequency matched on age and place of residence</t>
   </si>
   <si>
-    <t>detailed interview</t>
-  </si>
-  <si>
     <t xml:space="preserve">self-report, # sunburns as child and freq and duration of episodes of sun exposure per week. </t>
   </si>
   <si>
     <t xml:space="preserve">aspirin, ibuprofen, acetaminophen </t>
   </si>
   <si>
-    <t>reduced risk for NSAID use combined, excluding acetomenophin (OR 0.45, 0.222-0.92; p for trend &lt;0.05 decreasing melanoma risk with increasing NSAID use)</t>
+    <t>TOMS UVR measures linked at baseline</t>
+  </si>
+  <si>
+    <t>RCT 2x2</t>
+  </si>
+  <si>
+    <t>100 mg aspirin</t>
+  </si>
+  <si>
+    <t>39,876. 100 mg aspirin every other day (19934) placebo (19942)</t>
+  </si>
+  <si>
+    <t>3,242 melanoma cases, 1,974 SCC cases, 178,655 controls</t>
+  </si>
+  <si>
+    <t>69,810 men 76,303 women, melanoma analysis combined genders</t>
+  </si>
+  <si>
+    <t>age, BMI, smoking, alcohol (&lt; 1 or &gt;=1 drink per week), family history of breast colorectal or ovarian</t>
+  </si>
+  <si>
+    <t>Avg Entry Age</t>
+  </si>
+  <si>
+    <t>Study population (n)</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>Mean 54.6 years  (7.0 SD)</t>
+  </si>
+  <si>
+    <t>Follow-up (yr)</t>
+  </si>
+  <si>
+    <t>10.1 mean</t>
+  </si>
+  <si>
+    <t>12 median</t>
+  </si>
+  <si>
+    <r>
+      <t>regional solar radiation at clincal center sites in langleys (1 langley = 1 g-cal/cm</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Women's Health Initiative OS; USA</t>
+  </si>
+  <si>
+    <t>history of NMSC and MSC, age, education, BMI, smoking, vitamind D intake, physical activity, skin type, sun exposure history, sunscreen use, regional solar radiation, time since last medical visit, medical indication for NSAID use</t>
+  </si>
+  <si>
+    <t>aspirin and non-ASA NSAIDS</t>
+  </si>
+  <si>
+    <t>59,806 postmenopausal Caucasian women ages 50-79</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Mean 54 for cases, 53 for controls</t>
+  </si>
+  <si>
+    <t>detailed interview, Sloan Kettering and James Cancer Hospital, Columbus OH</t>
+  </si>
+  <si>
+    <t>Dutch registry based, PHARMO and PALGA databases, 1991-2004</t>
+  </si>
+  <si>
+    <t>1,318 cases and 6,786 controls matched on DOB, gender and geographical region</t>
+  </si>
+  <si>
+    <t>Mean 55.3 for cases, 55.9 for controls</t>
+  </si>
+  <si>
+    <t>results not stratified by drug type, no geographical stratification, no control for statin use</t>
+  </si>
+  <si>
+    <t>age, gender, year of diagnosis, prior use of statins and estrogens, number? of ICD and ATC codes</t>
+  </si>
+  <si>
+    <t>low-dose aspirin exposure excluded in sub-group analyses, ~40% cases were in situ, no stratification across gender</t>
+  </si>
+  <si>
+    <t>geographical matching by pharmaceutical locations ~100</t>
+  </si>
+  <si>
+    <t>never exposed and &lt;2 years were combined because &lt;2 years exposure likely to not have effect on CM carcinogenesis and in prelim analysis showed no difference with never exposed on CM risk. Statins</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reduced risk in both genders with any long-term aspirin use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.57, 0.43-0.77)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, driven by continuous &lt;5 yr ASA use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.51, 0.35-0.75)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reduced risk in females </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.54, 0.30-0.99)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with consistent low-dose (30-100mg) aspirin over 3 years (&gt;= 990 pills), significant trend from no use to non-continuous use to continuous use observed in women (p=0.04)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reduced risk for NSAID use combined, excluding acetomenophin </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.45, 0.22-0.92)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; p for trend &lt;0.05 decreasing melanoma risk with increasing NSAID use)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">548 cases, reduced risk of melanoma with aspirin use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=0.79, 0.63-0.98)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; reduced melanoma risk with aspirin use &gt;5 yrs</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (HR=0.70 0.55-0.94)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no association. 68 cases on aspirin, 70 cases on placebo, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=0.97, 0.70-1.36)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">increased risk of melanoma for current aspirin users </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=1.32, 1.03-1.70)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no association; nsaid use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=1.12; 9% CI 0.84-1.48)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, regular or extra strength </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=1.22; 95%CI 0.76-1.58)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, non-aspirin NSAIDS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=1.22; 95% CI 0.75-1.99)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no association-- aspirin adjusted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=1.45, 0.44-4.74)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; non-aspirin NSAID adjusted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.71, 0.23-2.02)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -- adjusted for age, gnder, skin color, family hx of melanoma, # moles; COX-2 inhibitors </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.61, 0.28-1.31)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no association -- low dose </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=1.04, 0.88-1.22)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, current daily use (&lt;5 yr) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=0.99, 0.79-1.25)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, current daily use (&gt;= 5yrs) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=1.15, 0.83-1.59)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11 published studies included. Pooled data exposure 50-400 mg aspirin intake associated with reduced risk of all skin cancer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.94, 0.90-0.99)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Low-dose (&lt;150mg) reduce risk </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.95, 0.90-0.99)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. NO association with MELANOMA </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.96, 0.82-1.12)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 7 studies had information on melanoma, but these were significantly heterogeneous (p=0.00)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,6 +918,22 @@
     <font>
       <b/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -540,7 +1010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -569,9 +1039,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -580,6 +1047,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3530,71 +4012,78 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:IV4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.5703125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="62.7109375" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="15.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="30.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="22.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" style="4" customWidth="1"/>
+    <col min="13" max="13" width="45" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:13" s="14" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="14" t="s">
-        <v>7</v>
+      <c r="M1" s="17" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
@@ -3602,368 +4091,418 @@
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:11" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="1:13" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="8">
-        <v>59806</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" s="21"/>
+      <c r="H3" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="M3" s="20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>48</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>49</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>134</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="D5" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="I4" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>135</v>
+      <c r="F5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="M5" s="20" t="s">
+        <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>60</v>
+    <row r="6" spans="1:13" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>63</v>
+        <v>51</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:11" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F11" s="19">
+        <v>92125</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="8">
+        <v>68809</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="J17" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>81</v>
-      </c>
+    <row r="18" spans="1:11" s="7" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="K18" s="15"/>
     </row>
-    <row r="11" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" s="4">
-        <v>92125</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>77</v>
-      </c>
+    <row r="19" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="K19" s="16"/>
     </row>
-    <row r="12" spans="1:11" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="E12" s="7">
-        <v>68809</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:9" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="H17" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" s="7" customFormat="1" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I18" s="16"/>
-    </row>
-    <row r="19" spans="1:9" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="I19" s="17"/>
-    </row>
-    <row r="20" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F22" s="6"/>
+    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H22" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="48" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -3994,145 +4533,145 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -4160,7 +4699,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4172,31 +4711,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>73</v>
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lit review XLSX file, added 4 more papers to be read and filled out on spreadsheet
</commit_message>
<xml_diff>
--- a/references/Lit review_NSAIDS melanoma.xlsx
+++ b/references/Lit review_NSAIDS melanoma.xlsx
@@ -18,14 +18,14 @@
     <sheet name="strengths.limitations" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lit Review'!$A$1:$M$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Lit Review'!$A$1:$M$27</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="168">
   <si>
     <t>Study type</t>
   </si>
@@ -893,6 +893,45 @@
       </rPr>
       <t xml:space="preserve"> 7 studies had information on melanoma, but these were significantly heterogeneous (p=0.00)</t>
     </r>
+  </si>
+  <si>
+    <t>Brasky, 2014</t>
+  </si>
+  <si>
+    <t>Int J Cancer</t>
+  </si>
+  <si>
+    <t>Goodman, 2014</t>
+  </si>
+  <si>
+    <t>Cancer Prev Res</t>
+  </si>
+  <si>
+    <t>Increase in melanoma risk</t>
+  </si>
+  <si>
+    <t>Siiskonen, 2013</t>
+  </si>
+  <si>
+    <t>Eur J Clin Pharm</t>
+  </si>
+  <si>
+    <t>Dutch population, obtained from PALGA and linked to PHARMO, a drug dispensing network</t>
+  </si>
+  <si>
+    <t>Sorensen, 2003</t>
+  </si>
+  <si>
+    <t>BJC</t>
+  </si>
+  <si>
+    <t>Danish cancer registry</t>
+  </si>
+  <si>
+    <t>9 yrs</t>
+  </si>
+  <si>
+    <t>WHI</t>
   </si>
 </sst>
 </file>
@@ -4012,11 +4051,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4282,233 +4321,304 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+    <row r="8" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:13" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+    <row r="11" spans="1:13" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G11" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H11" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I11" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J11" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M11" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="13" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="8">
+        <v>68809</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="20" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:11" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E19" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F19" s="8">
         <v>92125</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="4" t="s">
+      <c r="G19" s="8"/>
+      <c r="H19" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J19" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="K19" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F12" s="8">
-        <v>68809</v>
-      </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>72</v>
-      </c>
+    <row r="20" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
     </row>
-    <row r="13" spans="1:13" ht="105" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="K13" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>96</v>
-      </c>
+    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
     </row>
-    <row r="14" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M14" s="7" t="s">
-        <v>105</v>
-      </c>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
     </row>
-    <row r="16" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J24" s="10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:11" s="7" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="25" spans="1:11" s="7" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B25" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="J18" s="15" t="s">
+      <c r="J25" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="K18" s="15"/>
+      <c r="K25" s="15"/>
     </row>
-    <row r="19" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="26" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J19" s="16" t="s">
+      <c r="J26" s="16" t="s">
         <v>154</v>
       </c>
-      <c r="K19" s="16"/>
+      <c r="K26" s="16"/>
     </row>
-    <row r="20" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H22" s="6"/>
+    <row r="27" spans="1:11" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="48" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
-    <brk id="8" max="16383" man="1"/>
-    <brk id="16" max="10" man="1"/>
+    <brk id="9" max="16383" man="1"/>
+    <brk id="23" max="10" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
lit review XLSX file, finished brasky and johannesdottier
</commit_message>
<xml_diff>
--- a/references/Lit review_NSAIDS melanoma.xlsx
+++ b/references/Lit review_NSAIDS melanoma.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="176">
   <si>
     <t>Study type</t>
   </si>
@@ -180,18 +180,12 @@
     <t>Drugs studied</t>
   </si>
   <si>
-    <t>all nsaids</t>
-  </si>
-  <si>
     <t>both</t>
   </si>
   <si>
     <t>aspirin and other nsaids</t>
   </si>
   <si>
-    <t>reduced risk of SCC and malignant melanoma with different NSAID use; greater risk reduction with greater duration and dosage of NSAID use</t>
-  </si>
-  <si>
     <t>no information on skin type and sun exposure</t>
   </si>
   <si>
@@ -378,15 +372,15 @@
     <t>RCT 2x2</t>
   </si>
   <si>
+    <t>Follow-up</t>
+  </si>
+  <si>
     <t>100 mg aspirin</t>
   </si>
   <si>
     <t>39,876. 100 mg aspirin every other day (19934) placebo (19942)</t>
   </si>
   <si>
-    <t>3,242 melanoma cases, 1,974 SCC cases, 178,655 controls</t>
-  </si>
-  <si>
     <t>69,810 men 76,303 women, melanoma analysis combined genders</t>
   </si>
   <si>
@@ -403,15 +397,6 @@
   </si>
   <si>
     <t>Mean 54.6 years  (7.0 SD)</t>
-  </si>
-  <si>
-    <t>Follow-up (yr)</t>
-  </si>
-  <si>
-    <t>10.1 mean</t>
-  </si>
-  <si>
-    <t>12 median</t>
   </si>
   <si>
     <r>
@@ -931,7 +916,134 @@
     <t>9 yrs</t>
   </si>
   <si>
-    <t>WHI</t>
+    <t>9.7 yrs</t>
+  </si>
+  <si>
+    <t>10.1 mean yrs</t>
+  </si>
+  <si>
+    <t>12 median yrs</t>
+  </si>
+  <si>
+    <t>Women's Health Initiative</t>
+  </si>
+  <si>
+    <t>all nsaids categorized as none, inconsistent, and consistent</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reduced melanoma risk, no aspirin vs any consistent aspirin use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=0.66, 0.46-0.95)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, no reduction in all NSAIDS and non-aspirin NSAIDS</t>
+    </r>
+  </si>
+  <si>
+    <t>531 melanoma cases, out of 129,013 participants</t>
+  </si>
+  <si>
+    <t>Measurement of NSAIDS:  limited data on non-aspirin dose, no data on frequency of NSAID use</t>
+  </si>
+  <si>
+    <t>no direct UVR measure, controlled for US region and physical activity</t>
+  </si>
+  <si>
+    <t>NSAID use categorized into none (non-use at baseline and year 3), inconsistent (use at baseline or year 3), and consistent (use at both baseline and year 3); NSAID duration among consistent users only, &lt;5 or &gt;=5 years</t>
+  </si>
+  <si>
+    <t>matched by count of residence, no direct UVR measure</t>
+  </si>
+  <si>
+    <t>3,242 melanoma cases, 1,974 SCC cases; 178,655 controls</t>
+  </si>
+  <si>
+    <t>all nsaids, low and high dose aspirin, COX-inhibitors</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reduced risk of SCC </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(IRR=0.85 0.76-0.94)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and malignant melanoma </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(IRR=0.87, 0.80-0.95)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with ever NSAID use; greater melanoma risk reduction </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(IRR=0.54, 0.38-0.75)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with greater duration (7+ years) and dosage (25%+ coverage of total duration of NSAID use)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -4055,7 +4167,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4063,7 +4175,7 @@
     <col min="1" max="1" width="20.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11" style="4" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="22" style="4" customWidth="1"/>
     <col min="7" max="7" width="17" style="4" customWidth="1"/>
@@ -4087,16 +4199,16 @@
         <v>0</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="E1" s="17" t="s">
         <v>49</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H1" s="17" t="s">
         <v>46</v>
@@ -4105,10 +4217,10 @@
         <v>50</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K1" s="17" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L1" s="17" t="s">
         <v>1</v>
@@ -4119,7 +4231,7 @@
     </row>
     <row r="2" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -4144,154 +4256,154 @@
         <v>5</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="21" t="s">
         <v>128</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>133</v>
       </c>
       <c r="G3" s="21"/>
       <c r="H3" s="20" t="s">
         <v>47</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="J3" s="20" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="K3" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>47</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="H5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="M5" s="20" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="J6" s="7" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
@@ -4300,203 +4412,230 @@
         <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>119</v>
+        <v>173</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>51</v>
+        <v>174</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>54</v>
+        <v>175</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="1:13" s="7" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>167</v>
       </c>
+      <c r="K8" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>171</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="J11" s="7" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F13" s="8">
         <v>68809</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="I13" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="J13" s="7" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="E14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="H14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>94</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" s="7" t="s">
+      <c r="F15" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="J15" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K15" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="7" t="s">
+      <c r="L15" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M15" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="K15" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="20" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C16" s="20" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:11" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -4510,37 +4649,37 @@
         <v>5</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F19" s="8">
         <v>92125</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J19" s="7" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -4556,54 +4695,54 @@
     <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="7" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="K25" s="15"/>
     </row>
     <row r="26" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="C26" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J26" s="16" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K26" s="16"/>
     </row>
     <row r="27" spans="1:11" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -4821,34 +4960,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
file clean up, moved files in sample dir to references dir, moved QC forms to QC dir and deleted models.2.w.sas file
</commit_message>
<xml_diff>
--- a/references/Lit review_NSAIDS melanoma.xlsx
+++ b/references/Lit review_NSAIDS melanoma.xlsx
@@ -20,12 +20,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Lit Review'!$A$1:$M$27</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="196">
   <si>
     <t>Study type</t>
   </si>
@@ -186,9 +186,6 @@
     <t>aspirin and other nsaids</t>
   </si>
   <si>
-    <t>no information on skin type and sun exposure</t>
-  </si>
-  <si>
     <t>aspirin</t>
   </si>
   <si>
@@ -225,9 +222,6 @@
     <t>female</t>
   </si>
   <si>
-    <t>pathology reports were missing for some cases; the study population only consisted of caucasian nurses</t>
-  </si>
-  <si>
     <t>J American Academy of Dermatology</t>
   </si>
   <si>
@@ -315,9 +309,6 @@
     <t>structured interview and aspirin use have have been misreported, small numbers</t>
   </si>
   <si>
-    <t>Nurses Health Study</t>
-  </si>
-  <si>
     <t>Cutaneous Melanoma cases more likely to have light hair, eyes, number of freckles, skin response to sun and number of sunburns</t>
   </si>
   <si>
@@ -339,9 +330,6 @@
     <t>age, sex, race, education, smoking, BMI, physical activity, HRT use, hx mammogram, hx of colorectal endoscopy, hx PSA testing, use of nonaspirin NSAIDs, hx heart attack, diabetes, hypertension</t>
   </si>
   <si>
-    <t>Vitamins and Lifestyle (VITAL) cohort</t>
-  </si>
-  <si>
     <t>Genes, Environment, and Melanoma case-control</t>
   </si>
   <si>
@@ -376,9 +364,6 @@
   </si>
   <si>
     <t>100 mg aspirin</t>
-  </si>
-  <si>
-    <t>39,876. 100 mg aspirin every other day (19934) placebo (19942)</t>
   </si>
   <si>
     <t>69,810 men 76,303 women, melanoma analysis combined genders</t>
@@ -613,7 +598,543 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">increased risk of melanoma for current aspirin users </t>
+      <t xml:space="preserve">no association-- aspirin adjusted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=1.45, 0.44-4.74)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">; non-aspirin NSAID adjusted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.71, 0.23-2.02)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> -- adjusted for age, gnder, skin color, family hx of melanoma, # moles; COX-2 inhibitors </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.61, 0.28-1.31)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no association -- low dose </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=1.04, 0.88-1.22)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, current daily use (&lt;5 yr) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=0.99, 0.79-1.25)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, current daily use (&gt;= 5yrs) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=1.15, 0.83-1.59)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">11 published studies included. Pooled data exposure 50-400 mg aspirin intake associated with reduced risk of all skin cancer </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.94, 0.90-0.99)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Low-dose (&lt;150mg) reduce risk </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.95, 0.90-0.99)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. NO association with MELANOMA </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(OR=0.96, 0.82-1.12)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 7 studies had information on melanoma, but these were significantly heterogeneous (p=0.00)</t>
+    </r>
+  </si>
+  <si>
+    <t>Brasky, 2014</t>
+  </si>
+  <si>
+    <t>Int J Cancer</t>
+  </si>
+  <si>
+    <t>Goodman, 2014</t>
+  </si>
+  <si>
+    <t>Cancer Prev Res</t>
+  </si>
+  <si>
+    <t>Increase in melanoma risk</t>
+  </si>
+  <si>
+    <t>Siiskonen, 2013</t>
+  </si>
+  <si>
+    <t>Eur J Clin Pharm</t>
+  </si>
+  <si>
+    <t>Sorensen, 2003</t>
+  </si>
+  <si>
+    <t>BJC</t>
+  </si>
+  <si>
+    <t>9.7 yrs</t>
+  </si>
+  <si>
+    <t>10.1 mean yrs</t>
+  </si>
+  <si>
+    <t>12 median yrs</t>
+  </si>
+  <si>
+    <t>Women's Health Initiative</t>
+  </si>
+  <si>
+    <t>all nsaids categorized as none, inconsistent, and consistent</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reduced melanoma risk, no aspirin vs any consistent aspirin use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=0.66, 0.46-0.95)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, no reduction in all NSAIDS and non-aspirin NSAIDS</t>
+    </r>
+  </si>
+  <si>
+    <t>531 melanoma cases, out of 129,013 participants</t>
+  </si>
+  <si>
+    <t>Measurement of NSAIDS:  limited data on non-aspirin dose, no data on frequency of NSAID use</t>
+  </si>
+  <si>
+    <t>no direct UVR measure, controlled for US region and physical activity</t>
+  </si>
+  <si>
+    <t>NSAID use categorized into none (non-use at baseline and year 3), inconsistent (use at baseline or year 3), and consistent (use at both baseline and year 3); NSAID duration among consistent users only, &lt;5 or &gt;=5 years</t>
+  </si>
+  <si>
+    <t>matched by count of residence, no direct UVR measure</t>
+  </si>
+  <si>
+    <t>3,242 melanoma cases, 1,974 SCC cases; 178,655 controls</t>
+  </si>
+  <si>
+    <t>all nsaids, low and high dose aspirin, COX-inhibitors</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reduced risk of SCC </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(IRR=0.85 0.76-0.94)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and malignant melanoma </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(IRR=0.87, 0.80-0.95)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with ever NSAID use; greater melanoma risk reduction </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(IRR=0.54, 0.38-0.75)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with greater duration (7+ years) and dosage (25%+ coverage of total duration of NSAID use)</t>
+    </r>
+  </si>
+  <si>
+    <t>no information on skin type and sun exposure, no length of prescriptions so no daily or weekly doses of NSAIDs</t>
+  </si>
+  <si>
+    <t>Vitamins and Lifestyle (VITAL) cohort from western Washington State</t>
+  </si>
+  <si>
+    <t>349 cases of malignant melanoma identified from 68,809 participants</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no association; nsaid use </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=1.12; 0.84-1.48)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, regular or extra strength </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=1.10, 0.76-1.58)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, non-aspirin NSAIDS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(HR=1.22, 0.75-1.99)</t>
+    </r>
+  </si>
+  <si>
+    <t>has family history of melanoma, freckles, sunburns at young ages, reaction to sunlight, and hair color</t>
+  </si>
+  <si>
+    <t>68 cases on aspirin, 70 on placebo from 39,876. 100 mg aspirin every other day (19934) placebo (19942)</t>
+  </si>
+  <si>
+    <t>167 observed melanoma cases from 172,057 participants</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no difference in expected incidence </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(SIR=1.0, 0.8-1.1)</t>
+    </r>
+  </si>
+  <si>
+    <t>mean 47.2</t>
+  </si>
+  <si>
+    <t>aspirin (low 81mg, regular 325mg, and extra strength) and other nsaids</t>
+  </si>
+  <si>
+    <t>Danish cancer registry and North Jutland Prescription Database, 1989-1995</t>
+  </si>
+  <si>
+    <t>mean 5.4, 1 year after first prescription</t>
+  </si>
+  <si>
+    <t>Short follow-up time, no underlying indications for NSAID use or other diseases, no control for smoking, alcohol, diet, no data on drug compliance</t>
+  </si>
+  <si>
+    <t>lacking many- limitations</t>
+  </si>
+  <si>
+    <t>658 melanoma cases from 92,125 participants</t>
+  </si>
+  <si>
+    <t>aspirin in 1980, other NSAIDS and acetaminophen in 1990</t>
+  </si>
+  <si>
+    <t>mean 53.2 aspirin group</t>
+  </si>
+  <si>
+    <t>UV-B flux in Robertson-Berger units, count x 10^-4</t>
+  </si>
+  <si>
+    <t>Caucasian women in Nurses Health Study USA, 1980-2008</t>
+  </si>
+  <si>
+    <t>pathology reports were missing for some cases; the study population only consisted of caucasian nurses, no full duration of non-aspirin NSAIDs</t>
+  </si>
+  <si>
+    <t>reaction of skin to sun exposure, ability to tan, number of severe sunburns, number of moles on left arm, family history of melanoma, UV-B availability at state of residence, menopausal status and use of postmenopausal hormones, height, BMI, physical activity, smoking status, intake of vitamin C, intake of vitamin D</t>
+  </si>
+  <si>
+    <t>Dutch population, obtained from PALGA, a national pathology network, and linked to PHARMO, a drug dispensing network</t>
+  </si>
+  <si>
+    <t>1,318 cases and 6,786 controls</t>
+  </si>
+  <si>
+    <t>mean 55.3 cases, mean 55.9 controls</t>
+  </si>
+  <si>
+    <t>propionic acid derivate NSAIDs, quinolones</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">no increased risk for past aspirin </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=1.29, 0.98-1.71)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or nonaspirin NSAIDS past </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(RR=0.91, 0.71-1.17)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ; increased risk of melanoma for current aspirin users </t>
     </r>
     <r>
       <rPr>
@@ -629,7 +1150,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">no association; nsaid use </t>
+      <t xml:space="preserve">Propionic acid derivative NSAIDS (Ibuprofen) showed increased risk </t>
     </r>
     <r>
       <rPr>
@@ -640,410 +1161,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(HR=1.12; 9% CI 0.84-1.48)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, regular or extra strength </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(HR=1.22; 95%CI 0.76-1.58)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, non-aspirin NSAIDS </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(HR=1.22; 95% CI 0.75-1.99)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">no association-- aspirin adjusted </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(OR=1.45, 0.44-4.74)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">; non-aspirin NSAID adjusted </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(OR=0.71, 0.23-2.02)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> -- adjusted for age, gnder, skin color, family hx of melanoma, # moles; COX-2 inhibitors </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(OR=0.61, 0.28-1.31)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">no association -- low dose </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(RR=1.04, 0.88-1.22)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, current daily use (&lt;5 yr) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(RR=0.99, 0.79-1.25)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, current daily use (&gt;= 5yrs) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(RR=1.15, 0.83-1.59)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">11 published studies included. Pooled data exposure 50-400 mg aspirin intake associated with reduced risk of all skin cancer </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(OR=0.94, 0.90-0.99)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. Low-dose (&lt;150mg) reduce risk </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(OR=0.95, 0.90-0.99)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. NO association with MELANOMA </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(OR=0.96, 0.82-1.12)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 7 studies had information on melanoma, but these were significantly heterogeneous (p=0.00)</t>
-    </r>
-  </si>
-  <si>
-    <t>Brasky, 2014</t>
-  </si>
-  <si>
-    <t>Int J Cancer</t>
-  </si>
-  <si>
-    <t>Goodman, 2014</t>
-  </si>
-  <si>
-    <t>Cancer Prev Res</t>
-  </si>
-  <si>
-    <t>Increase in melanoma risk</t>
-  </si>
-  <si>
-    <t>Siiskonen, 2013</t>
-  </si>
-  <si>
-    <t>Eur J Clin Pharm</t>
-  </si>
-  <si>
-    <t>Dutch population, obtained from PALGA and linked to PHARMO, a drug dispensing network</t>
-  </si>
-  <si>
-    <t>Sorensen, 2003</t>
-  </si>
-  <si>
-    <t>BJC</t>
-  </si>
-  <si>
-    <t>Danish cancer registry</t>
-  </si>
-  <si>
-    <t>9 yrs</t>
-  </si>
-  <si>
-    <t>9.7 yrs</t>
-  </si>
-  <si>
-    <t>10.1 mean yrs</t>
-  </si>
-  <si>
-    <t>12 median yrs</t>
-  </si>
-  <si>
-    <t>Women's Health Initiative</t>
-  </si>
-  <si>
-    <t>all nsaids categorized as none, inconsistent, and consistent</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">reduced melanoma risk, no aspirin vs any consistent aspirin use </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(HR=0.66, 0.46-0.95)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, no reduction in all NSAIDS and non-aspirin NSAIDS</t>
-    </r>
-  </si>
-  <si>
-    <t>531 melanoma cases, out of 129,013 participants</t>
-  </si>
-  <si>
-    <t>Measurement of NSAIDS:  limited data on non-aspirin dose, no data on frequency of NSAID use</t>
-  </si>
-  <si>
-    <t>no direct UVR measure, controlled for US region and physical activity</t>
-  </si>
-  <si>
-    <t>NSAID use categorized into none (non-use at baseline and year 3), inconsistent (use at baseline or year 3), and consistent (use at both baseline and year 3); NSAID duration among consistent users only, &lt;5 or &gt;=5 years</t>
-  </si>
-  <si>
-    <t>matched by count of residence, no direct UVR measure</t>
-  </si>
-  <si>
-    <t>3,242 melanoma cases, 1,974 SCC cases; 178,655 controls</t>
-  </si>
-  <si>
-    <t>all nsaids, low and high dose aspirin, COX-inhibitors</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">reduced risk of SCC </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(IRR=0.85 0.76-0.94)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and malignant melanoma </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(IRR=0.87, 0.80-0.95)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> with ever NSAID use; greater melanoma risk reduction </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(IRR=0.54, 0.38-0.75)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> with greater duration (7+ years) and dosage (25%+ coverage of total duration of NSAID use)</t>
-    </r>
+      <t>(OR=1.33, 1.14-1.54)</t>
+    </r>
+  </si>
+  <si>
+    <t>photoxic drug use astertainment duration might have been too short being 3 years prior to diganosis of CM, no duration of drug use prior to 3 years</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>no life-style factors, no family history of melanoma or melanoma specific risk factors</t>
   </si>
 </sst>
 </file>
@@ -1193,12 +1321,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1213,6 +1335,12 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4165,9 +4293,9 @@
   </sheetPr>
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4175,7 +4303,7 @@
     <col min="1" max="1" width="20.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="23.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="22" style="4" customWidth="1"/>
     <col min="7" max="7" width="17" style="4" customWidth="1"/>
@@ -4189,49 +4317,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="14" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="17" t="s">
+      <c r="I1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="J1" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="13" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
@@ -4245,104 +4373,104 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
     </row>
-    <row r="3" spans="1:13" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+    <row r="3" spans="1:13" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>164</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="20" t="s">
+      <c r="D3" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="20" t="s">
-        <v>127</v>
-      </c>
-      <c r="J3" s="20" t="s">
-        <v>143</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>126</v>
+      <c r="I3" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="J3" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>47</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>48</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>51</v>
@@ -4351,36 +4479,36 @@
         <v>52</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>136</v>
+        <v>133</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="7" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>51</v>
@@ -4389,21 +4517,21 @@
         <v>52</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L6" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
@@ -4412,340 +4540,400 @@
         <v>48</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>172</v>
+        <v>165</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="L7" s="18" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="7" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>47</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="J8" s="7" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K8" s="7" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="L8" s="7" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>64</v>
       </c>
+      <c r="I11" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="7" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" s="7" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>89</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" s="8">
-        <v>68809</v>
+        <v>167</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>168</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="7" t="s">
         <v>51</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>52</v>
+        <v>175</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>146</v>
+        <v>169</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="E14" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>51</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:13" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>51</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="18" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="J16" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="M16" s="18" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="7" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="M17" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:13" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="L15" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="20" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:11" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="7" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F19" s="8">
-        <v>92125</v>
-      </c>
-      <c r="G19" s="8"/>
-      <c r="H19" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>155</v>
-      </c>
       <c r="B20" s="4" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
+        <v>187</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>195</v>
+      </c>
     </row>
-    <row r="21" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
     </row>
-    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:11" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:13" s="10" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="7" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="7" customFormat="1" ht="194.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25" s="20"/>
+    </row>
+    <row r="26" spans="1:13" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="J25" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="K25" s="15"/>
+      <c r="J26" s="21" t="s">
+        <v>142</v>
+      </c>
+      <c r="K26" s="21"/>
     </row>
-    <row r="26" spans="1:11" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="K26" s="16"/>
+    <row r="27" spans="1:13" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="27" spans="1:11" s="7" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H29" s="6"/>
     </row>
   </sheetData>
@@ -4960,34 +5148,34 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>